<commit_message>
Sales Report and Call Monitoring Screen
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateSales.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateSales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MbuleloD\source\repos\udminsure\UDM.Insurance.Interface\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DaneB\source\repos\Insure\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448D114A-E8A0-479B-A7F7-5D32CA42945A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B234F30D-2D46-4D63-B8EF-3EFE7ADD72DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -44,28 +44,30 @@
     <definedName name="GrandTotalUnitsCF2" localSheetId="4">CarriedForwards!$D$10</definedName>
     <definedName name="Premium">Report!$E$7</definedName>
     <definedName name="PremiumCF2" localSheetId="4">CarriedForwards!$C$7</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Report!$A$1:$V$15</definedName>
+    <definedName name="Reason">Report!$J$7</definedName>
     <definedName name="ReferralResult">Report!$I$7</definedName>
     <definedName name="RefNo">Report!$C$7</definedName>
     <definedName name="RefNoCF2" localSheetId="4">CarriedForwards!#REF!</definedName>
-    <definedName name="RPBatch">Report!$L$7</definedName>
-    <definedName name="RPCampaign">Report!$K$5</definedName>
-    <definedName name="RPClient">Report!$N$7</definedName>
-    <definedName name="RPDateOfSale">Report!$K$7</definedName>
-    <definedName name="RPFallOffPremium">Report!$Q$7</definedName>
-    <definedName name="RPGrandTotalFallOffPremium">Report!$Q$10</definedName>
-    <definedName name="RPGrandTotalOriginalPremium">Report!$O$10</definedName>
-    <definedName name="RPGrandTotalReducedPremium">Report!$P$10</definedName>
-    <definedName name="RPGrandTotalSales">Report!$M$10</definedName>
-    <definedName name="RPGrandTotalUnits">Report!$R$10</definedName>
-    <definedName name="RPOriginalPremium">Report!$O$7</definedName>
-    <definedName name="RPReducedPremium">Report!$P$7</definedName>
-    <definedName name="RPRefno">Report!$M$7</definedName>
-    <definedName name="RPTotalFallOffPremium">Report!$Q$8</definedName>
-    <definedName name="RPTotalOriginalPremium">Report!$O$8</definedName>
-    <definedName name="RPTotalReducedPremium">Report!$P$8</definedName>
-    <definedName name="RPTotalSales">Report!$M$8</definedName>
-    <definedName name="RPTotalUnits">Report!$R$8</definedName>
-    <definedName name="RPUnits">Report!$R$7</definedName>
+    <definedName name="RPBatch">Report!$M$7</definedName>
+    <definedName name="RPCampaign">Report!$L$5</definedName>
+    <definedName name="RPClient">Report!$O$7</definedName>
+    <definedName name="RPDateOfSale">Report!$L$7</definedName>
+    <definedName name="RPFallOffPremium">Report!$R$7</definedName>
+    <definedName name="RPGrandTotalFallOffPremium">Report!$R$10</definedName>
+    <definedName name="RPGrandTotalOriginalPremium">Report!$P$10</definedName>
+    <definedName name="RPGrandTotalReducedPremium">Report!$Q$10</definedName>
+    <definedName name="RPGrandTotalSales">Report!$N$10</definedName>
+    <definedName name="RPGrandTotalUnits">Report!$S$10</definedName>
+    <definedName name="RPOriginalPremium">Report!$P$7</definedName>
+    <definedName name="RPReducedPremium">Report!$Q$7</definedName>
+    <definedName name="RPRefno">Report!$N$7</definedName>
+    <definedName name="RPTotalFallOffPremium">Report!$R$8</definedName>
+    <definedName name="RPTotalOriginalPremium">Report!$P$8</definedName>
+    <definedName name="RPTotalReducedPremium">Report!$Q$8</definedName>
+    <definedName name="RPTotalSales">Report!$N$8</definedName>
+    <definedName name="RPTotalUnits">Report!$S$8</definedName>
+    <definedName name="RPUnits">Report!$S$7</definedName>
     <definedName name="SalesDates">Report!$A$3</definedName>
     <definedName name="SalesDatesCF">CarriedForwards!$B$3</definedName>
     <definedName name="SalesDatesCF2" localSheetId="4">CarriedForwards!$B$3</definedName>
@@ -86,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>Reference</t>
   </si>
@@ -203,6 +205,9 @@
   </si>
   <si>
     <t>Referral Generated</t>
+  </si>
+  <si>
+    <t>Reason</t>
   </si>
 </sst>
 </file>
@@ -505,7 +510,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -645,16 +650,23 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -986,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,49 +1012,51 @@
     <col min="6" max="6" width="14.7109375" style="12" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
     <col min="8" max="9" width="16.7109375" style="24" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" style="24" customWidth="1"/>
-    <col min="11" max="12" width="18.7109375" customWidth="1"/>
-    <col min="13" max="13" width="24.7109375" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" style="24" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" customWidth="1"/>
-    <col min="17" max="17" width="18.7109375" style="24" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="43.140625" style="24" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" style="24" customWidth="1"/>
+    <col min="12" max="13" width="18.7109375" customWidth="1"/>
+    <col min="14" max="14" width="24.7109375" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" style="24" customWidth="1"/>
+    <col min="17" max="17" width="18.7109375" customWidth="1"/>
+    <col min="18" max="18" width="18.7109375" style="24" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="63" t="s">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
       <c r="I5" s="58"/>
-      <c r="K5" s="62" t="s">
+      <c r="J5" s="62"/>
+      <c r="L5" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="62"/>
-      <c r="O5" s="62"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="62"/>
-      <c r="R5" s="62"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M5" s="66"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="66"/>
+      <c r="P5" s="66"/>
+      <c r="Q5" s="66"/>
+      <c r="R5" s="66"/>
+      <c r="S5" s="67"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
@@ -1070,32 +1084,35 @@
       <c r="I6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="J6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="M6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="N6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="O6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="P6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="Q6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="R6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="S6" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1105,16 +1122,17 @@
       <c r="G7" s="42"/>
       <c r="H7" s="40"/>
       <c r="I7" s="59"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="3"/>
+      <c r="J7" s="63"/>
+      <c r="L7" s="2"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
-      <c r="O7" s="4"/>
+      <c r="O7" s="3"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
-      <c r="R7" s="13"/>
-    </row>
-    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R7" s="4"/>
+      <c r="S7" s="13"/>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="6"/>
       <c r="E8" s="5"/>
       <c r="F8" s="14"/>
@@ -1122,24 +1140,25 @@
         <v>35</v>
       </c>
       <c r="I8" s="60"/>
-      <c r="K8" s="24"/>
+      <c r="J8" s="61"/>
       <c r="L8" s="24"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="5"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="24"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
-      <c r="R8" s="14"/>
-    </row>
-    <row r="9" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="K9" s="24"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="14"/>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="L9" s="24"/>
       <c r="M9" s="24"/>
       <c r="N9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="R9" s="25"/>
-    </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="S9" s="25"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
         <v>6</v>
       </c>
@@ -1150,32 +1169,33 @@
         <v>35</v>
       </c>
       <c r="I10" s="60"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="23" t="s">
+      <c r="J10" s="61"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="M10" s="9"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="10"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="24"/>
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
-      <c r="R10" s="15"/>
-    </row>
-    <row r="11" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:18" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R10" s="10"/>
+      <c r="S10" s="15"/>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F12" s="25"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="61" t="s">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61" t="s">
+      <c r="C13" s="64"/>
+      <c r="D13" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="61"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E13" s="64"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
       <c r="B14" s="26" t="s">
         <v>13</v>
@@ -1190,7 +1210,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>15</v>
       </c>
@@ -1205,8 +1225,8 @@
   <mergeCells count="4">
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:E13"/>
-    <mergeCell ref="K5:R5"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="L5:S5"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1228,10 +1248,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="66"/>
+      <c r="B1" s="69"/>
       <c r="C1" s="18"/>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
@@ -1248,10 +1268,10 @@
       <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="67"/>
+      <c r="B3" s="70"/>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
@@ -1409,13 +1429,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="73"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="76"/>
     </row>
     <row r="2" spans="1:5" s="25" customFormat="1" ht="6.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="31"/>
@@ -1425,27 +1445,27 @@
       <c r="E2" s="31"/>
     </row>
     <row r="3" spans="1:5" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="74"/>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
+      <c r="A3" s="77"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
     </row>
     <row r="4" spans="1:5" s="25" customFormat="1" ht="6.95" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:5" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="74"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
     </row>
     <row r="6" spans="1:5" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="68"/>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="70"/>
+      <c r="A7" s="71"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="73"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -1472,13 +1492,13 @@
       <c r="E9" s="32"/>
     </row>
     <row r="10" spans="1:5" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="76"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="77"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="80"/>
     </row>
     <row r="11" spans="1:5" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:5" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -1526,16 +1546,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="80"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="83"/>
     </row>
     <row r="2" spans="1:8" s="25" customFormat="1" ht="6.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="31"/>
@@ -1547,34 +1567,34 @@
       <c r="G2" s="31"/>
     </row>
     <row r="3" spans="1:8" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="74"/>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
+      <c r="A3" s="77"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
     </row>
     <row r="4" spans="1:8" s="25" customFormat="1" ht="6.95" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:8" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="74"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
     </row>
     <row r="6" spans="1:8" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="68"/>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="81"/>
+      <c r="A7" s="71"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="84"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -1613,16 +1633,16 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" s="25" customFormat="1" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="76"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="81"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="84"/>
     </row>
     <row r="11" spans="1:8" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:8" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -1669,7 +1689,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B74D4BE-249A-401F-AC30-6DB979373A56}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1692,12 +1714,12 @@
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="81"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="84"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>

</xml_diff>

<commit_message>
Debi check details update
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateSales.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateSales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DaneB\source\repos\Insure\UDM.Insurance.Interface\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TyronR\Desktop\Source\udminsure\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF44CE3-330C-4C01-A3BE-E0998956CDEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C532695D-48B5-4DAD-A4CC-789B882004C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,7 @@
     <definedName name="GrandTotalCarriedForwardsBase">Report!$B$15</definedName>
     <definedName name="GrandTotalCarriedForwardUnits">Report!$E$15</definedName>
     <definedName name="GrandTotalCarriedForwardUpgrades">Report!$D$15</definedName>
+    <definedName name="GrandTotalIncentive">Report!$K$10</definedName>
     <definedName name="GrandTotalPremium">Report!$E$10</definedName>
     <definedName name="GrandTotalPremiumCF2" localSheetId="4">CarriedForwards!$C$10</definedName>
     <definedName name="GrandTotalReferrals">Report!$I$10</definedName>
@@ -42,37 +43,40 @@
     <definedName name="GrandTotalSalesCF2" localSheetId="4">CarriedForwards!$B$10</definedName>
     <definedName name="GrandTotalUnits">Report!$F$10</definedName>
     <definedName name="GrandTotalUnitsCF2" localSheetId="4">CarriedForwards!$D$10</definedName>
+    <definedName name="Incentive">Report!$K$7</definedName>
+    <definedName name="MandateStatus">Report!$J$7</definedName>
     <definedName name="Premium">Report!$E$7</definedName>
     <definedName name="PremiumCF2" localSheetId="4">CarriedForwards!$C$7</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Report!$A$1:$V$15</definedName>
-    <definedName name="Reason">Report!$J$7</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Report!$A$1:$X$15</definedName>
+    <definedName name="Reason">Report!$L$7</definedName>
     <definedName name="ReferralResult">Report!$I$7</definedName>
     <definedName name="RefNo">Report!$C$7</definedName>
     <definedName name="RefNoCF2" localSheetId="4">CarriedForwards!#REF!</definedName>
-    <definedName name="RPBatch">Report!$M$7</definedName>
-    <definedName name="RPCampaign">Report!$L$5</definedName>
-    <definedName name="RPClient">Report!$O$7</definedName>
-    <definedName name="RPDateOfSale">Report!$L$7</definedName>
-    <definedName name="RPFallOffPremium">Report!$R$7</definedName>
-    <definedName name="RPGrandTotalFallOffPremium">Report!$R$10</definedName>
-    <definedName name="RPGrandTotalOriginalPremium">Report!$P$10</definedName>
-    <definedName name="RPGrandTotalReducedPremium">Report!$Q$10</definedName>
-    <definedName name="RPGrandTotalSales">Report!$N$10</definedName>
-    <definedName name="RPGrandTotalUnits">Report!$S$10</definedName>
-    <definedName name="RPOriginalPremium">Report!$P$7</definedName>
-    <definedName name="RPReducedPremium">Report!$Q$7</definedName>
-    <definedName name="RPRefno">Report!$N$7</definedName>
-    <definedName name="RPTotalFallOffPremium">Report!$R$8</definedName>
-    <definedName name="RPTotalOriginalPremium">Report!$P$8</definedName>
-    <definedName name="RPTotalReducedPremium">Report!$Q$8</definedName>
-    <definedName name="RPTotalSales">Report!$N$8</definedName>
-    <definedName name="RPTotalUnits">Report!$S$8</definedName>
-    <definedName name="RPUnits">Report!$S$7</definedName>
+    <definedName name="RPBatch">Report!$O$7</definedName>
+    <definedName name="RPCampaign">Report!$N$5</definedName>
+    <definedName name="RPClient">Report!$Q$7</definedName>
+    <definedName name="RPDateOfSale">Report!$N$7</definedName>
+    <definedName name="RPFallOffPremium">Report!$T$7</definedName>
+    <definedName name="RPGrandTotalFallOffPremium">Report!$T$10</definedName>
+    <definedName name="RPGrandTotalOriginalPremium">Report!$R$10</definedName>
+    <definedName name="RPGrandTotalReducedPremium">Report!$S$10</definedName>
+    <definedName name="RPGrandTotalSales">Report!$P$10</definedName>
+    <definedName name="RPGrandTotalUnits">Report!$U$10</definedName>
+    <definedName name="RPOriginalPremium">Report!$R$7</definedName>
+    <definedName name="RPReducedPremium">Report!$S$7</definedName>
+    <definedName name="RPRefno">Report!$P$7</definedName>
+    <definedName name="RPTotalFallOffPremium">Report!$T$8</definedName>
+    <definedName name="RPTotalOriginalPremium">Report!$R$8</definedName>
+    <definedName name="RPTotalReducedPremium">Report!$S$8</definedName>
+    <definedName name="RPTotalSales">Report!$P$8</definedName>
+    <definedName name="RPTotalUnits">Report!$U$8</definedName>
+    <definedName name="RPUnits">Report!$U$7</definedName>
     <definedName name="SalesDates">Report!$A$3</definedName>
     <definedName name="SalesDatesCF">CarriedForwards!$B$3</definedName>
     <definedName name="SalesDatesCF2" localSheetId="4">CarriedForwards!$B$3</definedName>
     <definedName name="SavedStatus">Report!$G$7</definedName>
     <definedName name="SavedStatusOriginalDOS">Report!$H$7</definedName>
+    <definedName name="TotalIncentive">Report!$K$8</definedName>
     <definedName name="TotalPremium">Report!$E$8</definedName>
     <definedName name="TotalPremiumCF2" localSheetId="4">CarriedForwards!$C$8</definedName>
     <definedName name="TotalReferrals">Report!$I$8</definedName>
@@ -88,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
   <si>
     <t>Reference</t>
   </si>
@@ -208,6 +212,12 @@
   </si>
   <si>
     <t>Reason</t>
+  </si>
+  <si>
+    <t>Mandate Status</t>
+  </si>
+  <si>
+    <t>Incentive</t>
   </si>
 </sst>
 </file>
@@ -510,7 +520,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -659,6 +669,9 @@
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1000,65 +1013,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="12" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="9" width="16.7109375" style="24" customWidth="1"/>
-    <col min="10" max="10" width="43.140625" style="24" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" style="24" customWidth="1"/>
-    <col min="12" max="13" width="18.7109375" customWidth="1"/>
-    <col min="14" max="14" width="24.7109375" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" style="24" customWidth="1"/>
-    <col min="17" max="17" width="18.7109375" customWidth="1"/>
-    <col min="18" max="18" width="18.7109375" style="24" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.59765625" customWidth="1"/>
+    <col min="2" max="3" width="24.73046875" customWidth="1"/>
+    <col min="4" max="5" width="18.59765625" customWidth="1"/>
+    <col min="6" max="6" width="14.73046875" style="12" customWidth="1"/>
+    <col min="7" max="7" width="16.73046875" customWidth="1"/>
+    <col min="8" max="11" width="16.73046875" style="24" customWidth="1"/>
+    <col min="12" max="12" width="43.1328125" style="24" customWidth="1"/>
+    <col min="13" max="13" width="19.3984375" style="24" customWidth="1"/>
+    <col min="14" max="15" width="18.73046875" customWidth="1"/>
+    <col min="16" max="16" width="24.73046875" customWidth="1"/>
+    <col min="17" max="17" width="18.73046875" customWidth="1"/>
+    <col min="18" max="18" width="18.73046875" style="24" customWidth="1"/>
+    <col min="19" max="19" width="18.73046875" customWidth="1"/>
+    <col min="20" max="20" width="18.73046875" style="24" customWidth="1"/>
+    <col min="21" max="21" width="12.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="67" t="s">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A5" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
       <c r="I5" s="58"/>
-      <c r="J5" s="62"/>
-      <c r="L5" s="67" t="s">
+      <c r="J5" s="66"/>
+      <c r="K5" s="66"/>
+      <c r="L5" s="62"/>
+      <c r="N5" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="68"/>
-      <c r="N5" s="68"/>
-      <c r="O5" s="68"/>
-      <c r="P5" s="68"/>
-      <c r="Q5" s="68"/>
-      <c r="R5" s="68"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="69"/>
+      <c r="Q5" s="69"/>
+      <c r="R5" s="69"/>
       <c r="S5" s="69"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5" s="69"/>
+      <c r="U5" s="70"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
@@ -1087,34 +1102,40 @@
         <v>38</v>
       </c>
       <c r="J6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="N6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="O6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="P6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="Q6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="P6" s="7" t="s">
+      <c r="R6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="Q6" s="7" t="s">
+      <c r="S6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="R6" s="7" t="s">
+      <c r="T6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="S6" s="7" t="s">
+      <c r="U6" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1124,17 +1145,19 @@
       <c r="G7" s="42"/>
       <c r="H7" s="40"/>
       <c r="I7" s="59"/>
-      <c r="J7" s="63"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="63"/>
+      <c r="N7" s="2"/>
       <c r="O7" s="3"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
       <c r="R7" s="4"/>
-      <c r="S7" s="64"/>
-    </row>
-    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="64"/>
+    </row>
+    <row r="8" spans="1:21" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C8" s="6"/>
       <c r="E8" s="5"/>
       <c r="F8" s="14"/>
@@ -1143,24 +1166,26 @@
       </c>
       <c r="I8" s="60"/>
       <c r="J8" s="61"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="6"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="61"/>
+      <c r="N8" s="24"/>
       <c r="O8" s="24"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="24"/>
       <c r="R8" s="5"/>
-      <c r="S8" s="65"/>
-    </row>
-    <row r="9" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="65"/>
+    </row>
+    <row r="9" spans="1:21" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="N9" s="24"/>
       <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
       <c r="Q9" s="24"/>
-      <c r="S9" s="25"/>
-    </row>
-    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S9" s="24"/>
+      <c r="U9" s="25"/>
+    </row>
+    <row r="10" spans="1:21" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B10" s="8" t="s">
         <v>6</v>
       </c>
@@ -1172,32 +1197,34 @@
       </c>
       <c r="I10" s="60"/>
       <c r="J10" s="61"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="23" t="s">
+      <c r="K10" s="60"/>
+      <c r="L10" s="61"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="N10" s="9"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="24"/>
       <c r="R10" s="10"/>
-      <c r="S10" s="15"/>
-    </row>
-    <row r="11" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="15"/>
+    </row>
+    <row r="11" spans="1:21" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="12" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.45">
       <c r="F12" s="25"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="66" t="s">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="B13" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66" t="s">
+      <c r="C13" s="67"/>
+      <c r="D13" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="66"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E13" s="67"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A14" s="24"/>
       <c r="B14" s="26" t="s">
         <v>13</v>
@@ -1212,7 +1239,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A15" s="27" t="s">
         <v>15</v>
       </c>
@@ -1228,7 +1255,7 @@
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="L5:S5"/>
+    <mergeCell ref="N5:U5"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1243,24 +1270,24 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:7" ht="21.4" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A1" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="71"/>
+      <c r="B1" s="72"/>
       <c r="C1" s="18"/>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -1269,18 +1296,18 @@
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="72" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="72"/>
+      <c r="B3" s="73"/>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -1289,7 +1316,7 @@
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="17" t="s">
         <v>8</v>
       </c>
@@ -1302,7 +1329,7 @@
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="19"/>
       <c r="B6" s="21"/>
       <c r="C6" s="16"/>
@@ -1311,7 +1338,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
     </row>
-    <row r="7" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="20" t="s">
         <v>11</v>
       </c>
@@ -1322,7 +1349,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A8" s="16"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -1331,7 +1358,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -1340,7 +1367,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -1349,7 +1376,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -1358,7 +1385,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -1367,7 +1394,7 @@
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="16"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -1376,7 +1403,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="16"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -1385,7 +1412,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -1394,7 +1421,7 @@
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="16"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -1420,56 +1447,56 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17" style="24" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="24" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" style="24" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="24"/>
+    <col min="2" max="2" width="14.3984375" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.59765625" style="24" customWidth="1"/>
+    <col min="4" max="4" width="21.59765625" style="24" customWidth="1"/>
+    <col min="5" max="5" width="24.86328125" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1328125" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="76" t="s">
+    <row r="1" spans="1:5" ht="25.9" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A1" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="78"/>
-    </row>
-    <row r="2" spans="1:5" s="25" customFormat="1" ht="6.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="79"/>
+    </row>
+    <row r="2" spans="1:5" s="25" customFormat="1" ht="6.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
       <c r="E2" s="31"/>
     </row>
-    <row r="3" spans="1:5" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="79"/>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-    </row>
-    <row r="4" spans="1:5" s="25" customFormat="1" ht="6.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:5" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="79"/>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-    </row>
-    <row r="6" spans="1:5" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="73"/>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="75"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A3" s="80"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+    </row>
+    <row r="4" spans="1:5" s="25" customFormat="1" ht="6.95" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A5" s="80"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+    </row>
+    <row r="6" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" s="74"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="76"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>24</v>
       </c>
@@ -1486,34 +1513,34 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A9" s="33"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="32"/>
     </row>
-    <row r="10" spans="1:5" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="80" t="s">
+    <row r="10" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A10" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="81"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="82"/>
-    </row>
-    <row r="11" spans="1:5" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:5" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:5" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:5" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:5" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:5" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="17" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="18" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="19" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="20" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="21" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="22" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="83"/>
+    </row>
+    <row r="11" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="17" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="18" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="19" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="20" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="21" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="22" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A7:E7"/>
@@ -1535,31 +1562,31 @@
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17" style="24" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="24" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="24" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" style="24" customWidth="1"/>
-    <col min="6" max="7" width="6.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" style="24" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="24"/>
+    <col min="2" max="2" width="14.3984375" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.59765625" style="24" customWidth="1"/>
+    <col min="4" max="4" width="26.3984375" style="24" customWidth="1"/>
+    <col min="5" max="5" width="6.1328125" style="24" customWidth="1"/>
+    <col min="6" max="7" width="6.1328125" style="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.1328125" style="24" customWidth="1"/>
+    <col min="9" max="16384" width="9.1328125" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="83" t="s">
+    <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.75">
+      <c r="A1" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="85"/>
-    </row>
-    <row r="2" spans="1:8" s="25" customFormat="1" ht="6.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="86"/>
+    </row>
+    <row r="2" spans="1:8" s="25" customFormat="1" ht="6.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
@@ -1568,37 +1595,37 @@
       <c r="F2" s="31"/>
       <c r="G2" s="31"/>
     </row>
-    <row r="3" spans="1:8" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="79"/>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-    </row>
-    <row r="4" spans="1:8" s="25" customFormat="1" ht="6.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:8" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="79"/>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-    </row>
-    <row r="6" spans="1:8" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="73"/>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="86"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A3" s="80"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+    </row>
+    <row r="4" spans="1:8" s="25" customFormat="1" ht="6.95" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:8" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A5" s="80"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+    </row>
+    <row r="6" spans="1:8" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" s="74"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="87"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>24</v>
       </c>
@@ -1624,7 +1651,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A9" s="33"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1634,20 +1661,20 @@
       <c r="G9" s="39"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" s="25" customFormat="1" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="80" t="s">
+    <row r="10" spans="1:8" s="25" customFormat="1" ht="13.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="81"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="86"/>
-    </row>
-    <row r="11" spans="1:8" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:8" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B10" s="82"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="87"/>
+    </row>
+    <row r="11" spans="1:8" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="1:8" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="D12" s="35" t="s">
         <v>30</v>
       </c>
@@ -1656,8 +1683,8 @@
       <c r="G12" s="34"/>
       <c r="H12" s="34"/>
     </row>
-    <row r="13" spans="1:8" s="25" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:8" s="25" customFormat="1" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="25" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="14" spans="1:8" s="25" customFormat="1" ht="13.9" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D14" s="36" t="s">
         <v>31</v>
       </c>
@@ -1666,14 +1693,14 @@
       <c r="G14" s="43"/>
       <c r="H14" s="38"/>
     </row>
-    <row r="15" spans="1:8" s="25" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:8" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="17" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="18" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="19" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="20" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="21" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="22" s="25" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:8" s="25" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="1:8" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="17" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="18" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="19" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="20" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="21" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="22" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A3:G3"/>
@@ -1695,33 +1722,33 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="24" customWidth="1"/>
-    <col min="2" max="3" width="18.5703125" style="24" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="25" customWidth="1"/>
-    <col min="5" max="5" width="48.7109375" style="24" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="24"/>
-    <col min="8" max="15" width="9.140625" style="44" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="24"/>
+    <col min="1" max="1" width="12.59765625" style="24" customWidth="1"/>
+    <col min="2" max="3" width="18.59765625" style="24" customWidth="1"/>
+    <col min="4" max="4" width="14.73046875" style="25" customWidth="1"/>
+    <col min="5" max="5" width="48.73046875" style="24" customWidth="1"/>
+    <col min="6" max="7" width="9.1328125" style="24"/>
+    <col min="8" max="15" width="9.1328125" style="44" customWidth="1"/>
+    <col min="16" max="16384" width="9.1328125" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B1" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="67" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B5" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="86"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="87"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
@@ -1731,7 +1758,7 @@
       <c r="N5" s="52"/>
       <c r="O5" s="52"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
@@ -1753,7 +1780,7 @@
       <c r="N6" s="45"/>
       <c r="O6" s="45"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B7" s="2"/>
       <c r="C7" s="4"/>
       <c r="D7" s="13"/>
@@ -1767,7 +1794,7 @@
       <c r="N7" s="48"/>
       <c r="O7" s="49"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="6"/>
       <c r="C8" s="5"/>
       <c r="D8" s="14"/>
@@ -1780,10 +1807,10 @@
       <c r="N8" s="51"/>
       <c r="O8" s="49"/>
     </row>
-    <row r="9" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="O9" s="49"/>
     </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="57" t="s">
         <v>6</v>
       </c>
@@ -1800,11 +1827,11 @@
       <c r="N10" s="53"/>
       <c r="O10" s="54"/>
     </row>
-    <row r="11" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:15" s="55" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:15" s="55" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:15" s="55" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:15" s="55" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:15" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="13" spans="1:15" s="55" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="14" spans="1:15" s="55" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="15" spans="1:15" s="55" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="16" spans="1:15" s="55" customFormat="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B5:E5"/>

</xml_diff>

<commit_message>
Sales Report Update Call Monitoring to Carried forward.
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateSales.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateSales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TyronR\Desktop\Source\udminsure\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C532695D-48B5-4DAD-A4CC-789B882004C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0906551D-37F7-4E25-B080-C54D53C62646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="RedeemedGiftsOLD" sheetId="4" r:id="rId3"/>
     <sheet name="RedeemedGifts" sheetId="5" r:id="rId4"/>
     <sheet name="CarriedForwards" sheetId="6" r:id="rId5"/>
+    <sheet name="ForwardToDCAgent" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="AgentName">Report!$A$1</definedName>
@@ -92,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
   <si>
     <t>Reference</t>
   </si>
@@ -218,6 +219,12 @@
   </si>
   <si>
     <t>Incentive</t>
+  </si>
+  <si>
+    <t>Forward To DC Agent</t>
+  </si>
+  <si>
+    <t>Reference Number</t>
   </si>
 </sst>
 </file>
@@ -520,7 +527,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -732,6 +739,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1015,39 +1030,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.59765625" customWidth="1"/>
-    <col min="2" max="3" width="24.73046875" customWidth="1"/>
-    <col min="4" max="5" width="18.59765625" customWidth="1"/>
-    <col min="6" max="6" width="14.73046875" style="12" customWidth="1"/>
-    <col min="7" max="7" width="16.73046875" customWidth="1"/>
-    <col min="8" max="11" width="16.73046875" style="24" customWidth="1"/>
-    <col min="12" max="12" width="43.1328125" style="24" customWidth="1"/>
-    <col min="13" max="13" width="19.3984375" style="24" customWidth="1"/>
-    <col min="14" max="15" width="18.73046875" customWidth="1"/>
-    <col min="16" max="16" width="24.73046875" customWidth="1"/>
-    <col min="17" max="17" width="18.73046875" customWidth="1"/>
-    <col min="18" max="18" width="18.73046875" style="24" customWidth="1"/>
-    <col min="19" max="19" width="18.73046875" customWidth="1"/>
-    <col min="20" max="20" width="18.73046875" style="24" customWidth="1"/>
-    <col min="21" max="21" width="12.73046875" customWidth="1"/>
+    <col min="1" max="1" width="18.6328125" customWidth="1"/>
+    <col min="2" max="3" width="24.7265625" customWidth="1"/>
+    <col min="4" max="5" width="18.6328125" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" customWidth="1"/>
+    <col min="8" max="11" width="16.7265625" style="24" customWidth="1"/>
+    <col min="12" max="12" width="43.08984375" style="24" customWidth="1"/>
+    <col min="13" max="13" width="19.36328125" style="24" customWidth="1"/>
+    <col min="14" max="15" width="18.7265625" customWidth="1"/>
+    <col min="16" max="16" width="24.7265625" customWidth="1"/>
+    <col min="17" max="17" width="18.7265625" customWidth="1"/>
+    <col min="18" max="18" width="18.7265625" style="24" customWidth="1"/>
+    <col min="19" max="19" width="18.7265625" customWidth="1"/>
+    <col min="20" max="20" width="18.7265625" style="24" customWidth="1"/>
+    <col min="21" max="21" width="12.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="68" t="s">
         <v>2</v>
       </c>
@@ -1073,7 +1088,7 @@
       <c r="T5" s="69"/>
       <c r="U5" s="70"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
@@ -1135,7 +1150,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1157,7 +1172,7 @@
       <c r="T7" s="4"/>
       <c r="U7" s="64"/>
     </row>
-    <row r="8" spans="1:21" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C8" s="6"/>
       <c r="E8" s="5"/>
       <c r="F8" s="14"/>
@@ -1177,7 +1192,7 @@
       <c r="T8" s="5"/>
       <c r="U8" s="65"/>
     </row>
-    <row r="9" spans="1:21" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="N9" s="24"/>
       <c r="O9" s="24"/>
       <c r="P9" s="24"/>
@@ -1185,7 +1200,7 @@
       <c r="S9" s="24"/>
       <c r="U9" s="25"/>
     </row>
-    <row r="10" spans="1:21" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="8" t="s">
         <v>6</v>
       </c>
@@ -1210,11 +1225,11 @@
       <c r="T10" s="10"/>
       <c r="U10" s="15"/>
     </row>
-    <row r="11" spans="1:21" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="12" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="F12" s="25"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B13" s="67" t="s">
         <v>17</v>
       </c>
@@ -1224,7 +1239,7 @@
       </c>
       <c r="E13" s="67"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="24"/>
       <c r="B14" s="26" t="s">
         <v>13</v>
@@ -1239,7 +1254,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="27" t="s">
         <v>15</v>
       </c>
@@ -1267,16 +1282,16 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21.4" thickBot="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:7" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="71" t="s">
         <v>10</v>
       </c>
@@ -1287,7 +1302,7 @@
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -1296,7 +1311,7 @@
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="73" t="s">
         <v>12</v>
       </c>
@@ -1307,7 +1322,7 @@
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -1316,7 +1331,7 @@
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>8</v>
       </c>
@@ -1329,7 +1344,7 @@
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="19"/>
       <c r="B6" s="21"/>
       <c r="C6" s="16"/>
@@ -1338,7 +1353,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
     </row>
-    <row r="7" spans="1:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="20" t="s">
         <v>11</v>
       </c>
@@ -1349,7 +1364,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
     </row>
-    <row r="8" spans="1:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A8" s="16"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -1358,7 +1373,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -1367,7 +1382,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -1376,7 +1391,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -1385,7 +1400,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -1394,7 +1409,7 @@
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="16"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -1403,7 +1418,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="16"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -1412,7 +1427,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -1421,7 +1436,7 @@
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="16"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -1436,6 +1451,7 @@
     <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1447,17 +1463,17 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17" style="24" customWidth="1"/>
-    <col min="2" max="2" width="14.3984375" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.59765625" style="24" customWidth="1"/>
-    <col min="4" max="4" width="21.59765625" style="24" customWidth="1"/>
-    <col min="5" max="5" width="24.86328125" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1328125" style="24"/>
+    <col min="2" max="2" width="14.36328125" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6328125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="21.6328125" style="24" customWidth="1"/>
+    <col min="5" max="5" width="24.81640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.08984375" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.9" thickBot="1" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="77" t="s">
         <v>25</v>
       </c>
@@ -1466,37 +1482,37 @@
       <c r="D1" s="78"/>
       <c r="E1" s="79"/>
     </row>
-    <row r="2" spans="1:5" s="25" customFormat="1" ht="6.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" s="25" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
       <c r="E2" s="31"/>
     </row>
-    <row r="3" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="80"/>
       <c r="B3" s="80"/>
       <c r="C3" s="80"/>
       <c r="D3" s="80"/>
       <c r="E3" s="80"/>
     </row>
-    <row r="4" spans="1:5" s="25" customFormat="1" ht="6.95" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" s="25" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:5" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="80"/>
       <c r="B5" s="80"/>
       <c r="C5" s="80"/>
       <c r="D5" s="80"/>
       <c r="E5" s="80"/>
     </row>
-    <row r="6" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="74"/>
       <c r="B7" s="75"/>
       <c r="C7" s="75"/>
       <c r="D7" s="75"/>
       <c r="E7" s="76"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>24</v>
       </c>
@@ -1513,14 +1529,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="33"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="32"/>
     </row>
-    <row r="10" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="81" t="s">
         <v>26</v>
       </c>
@@ -1529,18 +1545,18 @@
       <c r="D10" s="82"/>
       <c r="E10" s="83"/>
     </row>
-    <row r="11" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="1:5" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
-    <row r="17" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
-    <row r="18" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
-    <row r="19" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
-    <row r="20" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
-    <row r="21" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
-    <row r="22" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="11" spans="1:5" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:5" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:5" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:5" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:5" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:5" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="17" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="18" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="19" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="20" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="21" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="22" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A7:E7"/>
@@ -1562,19 +1578,19 @@
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17" style="24" customWidth="1"/>
-    <col min="2" max="2" width="14.3984375" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.59765625" style="24" customWidth="1"/>
-    <col min="4" max="4" width="26.3984375" style="24" customWidth="1"/>
-    <col min="5" max="5" width="6.1328125" style="24" customWidth="1"/>
-    <col min="6" max="7" width="6.1328125" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.1328125" style="24" customWidth="1"/>
-    <col min="9" max="16384" width="9.1328125" style="24"/>
+    <col min="2" max="2" width="14.36328125" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6328125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="26.36328125" style="24" customWidth="1"/>
+    <col min="5" max="5" width="6.08984375" style="24" customWidth="1"/>
+    <col min="6" max="7" width="6.08984375" style="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.08984375" style="24" customWidth="1"/>
+    <col min="9" max="16384" width="9.08984375" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.6">
       <c r="A1" s="84" t="s">
         <v>25</v>
       </c>
@@ -1586,7 +1602,7 @@
       <c r="G1" s="85"/>
       <c r="H1" s="86"/>
     </row>
-    <row r="2" spans="1:8" s="25" customFormat="1" ht="6.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" s="25" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
@@ -1595,7 +1611,7 @@
       <c r="F2" s="31"/>
       <c r="G2" s="31"/>
     </row>
-    <row r="3" spans="1:8" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="80"/>
       <c r="B3" s="80"/>
       <c r="C3" s="80"/>
@@ -1604,8 +1620,8 @@
       <c r="F3" s="80"/>
       <c r="G3" s="80"/>
     </row>
-    <row r="4" spans="1:8" s="25" customFormat="1" ht="6.95" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="1:8" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" s="25" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:8" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="80"/>
       <c r="B5" s="80"/>
       <c r="C5" s="80"/>
@@ -1614,8 +1630,8 @@
       <c r="F5" s="80"/>
       <c r="G5" s="80"/>
     </row>
-    <row r="6" spans="1:8" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="74"/>
       <c r="B7" s="75"/>
       <c r="C7" s="75"/>
@@ -1625,7 +1641,7 @@
       <c r="G7" s="75"/>
       <c r="H7" s="87"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>24</v>
       </c>
@@ -1651,7 +1667,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="33"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1661,7 +1677,7 @@
       <c r="G9" s="39"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" s="25" customFormat="1" ht="13.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" s="25" customFormat="1" ht="13.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="81" t="s">
         <v>26</v>
       </c>
@@ -1673,8 +1689,8 @@
       <c r="G10" s="82"/>
       <c r="H10" s="87"/>
     </row>
-    <row r="11" spans="1:8" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="1:8" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:8" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="D12" s="35" t="s">
         <v>30</v>
       </c>
@@ -1683,8 +1699,8 @@
       <c r="G12" s="34"/>
       <c r="H12" s="34"/>
     </row>
-    <row r="13" spans="1:8" s="25" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="14" spans="1:8" s="25" customFormat="1" ht="13.9" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" s="25" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:8" s="25" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D14" s="36" t="s">
         <v>31</v>
       </c>
@@ -1693,14 +1709,14 @@
       <c r="G14" s="43"/>
       <c r="H14" s="38"/>
     </row>
-    <row r="15" spans="1:8" s="25" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="1:8" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
-    <row r="17" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
-    <row r="18" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
-    <row r="19" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
-    <row r="20" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
-    <row r="21" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
-    <row r="22" s="25" customFormat="1" ht="13.15" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="1:8" s="25" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:8" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="17" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="18" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="19" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="20" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="21" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="22" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A3:G3"/>
@@ -1722,27 +1738,27 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.59765625" style="24" customWidth="1"/>
-    <col min="2" max="3" width="18.59765625" style="24" customWidth="1"/>
-    <col min="4" max="4" width="14.73046875" style="25" customWidth="1"/>
-    <col min="5" max="5" width="48.73046875" style="24" customWidth="1"/>
-    <col min="6" max="7" width="9.1328125" style="24"/>
-    <col min="8" max="15" width="9.1328125" style="44" customWidth="1"/>
-    <col min="16" max="16384" width="9.1328125" style="24"/>
+    <col min="1" max="1" width="12.6328125" style="24" customWidth="1"/>
+    <col min="2" max="3" width="18.6328125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="48.7265625" style="24" customWidth="1"/>
+    <col min="6" max="7" width="9.08984375" style="24"/>
+    <col min="8" max="15" width="9.08984375" style="44" customWidth="1"/>
+    <col min="16" max="16384" width="9.08984375" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B1" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B5" s="68" t="s">
         <v>36</v>
       </c>
@@ -1758,7 +1774,7 @@
       <c r="N5" s="52"/>
       <c r="O5" s="52"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
@@ -1780,7 +1796,7 @@
       <c r="N6" s="45"/>
       <c r="O6" s="45"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
       <c r="C7" s="4"/>
       <c r="D7" s="13"/>
@@ -1794,7 +1810,7 @@
       <c r="N7" s="48"/>
       <c r="O7" s="49"/>
     </row>
-    <row r="8" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="6"/>
       <c r="C8" s="5"/>
       <c r="D8" s="14"/>
@@ -1807,10 +1823,10 @@
       <c r="N8" s="51"/>
       <c r="O8" s="49"/>
     </row>
-    <row r="9" spans="1:15" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="O9" s="49"/>
     </row>
-    <row r="10" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="57" t="s">
         <v>6</v>
       </c>
@@ -1827,11 +1843,11 @@
       <c r="N10" s="53"/>
       <c r="O10" s="54"/>
     </row>
-    <row r="11" spans="1:15" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="13" spans="1:15" s="55" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="14" spans="1:15" s="55" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="15" spans="1:15" s="55" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="16" spans="1:15" s="55" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="11" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:15" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:15" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:15" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:15" s="55" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B5:E5"/>
@@ -1839,4 +1855,59 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{523127EF-725C-43E7-94D4-76A004FACF2B}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="4.81640625" style="92" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="71" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="72"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="89"/>
+      <c r="B2" s="16"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="73"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="89"/>
+      <c r="B4" s="16"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="90" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="91"/>
+      <c r="B6" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sales screen - Add Forward to DC Agent column
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateSales.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateSales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TyronR\Desktop\Source\udminsure\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0906551D-37F7-4E25-B080-C54D53C62646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0587364-4675-4C32-AFC3-0630F568C6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <definedName name="ClientCF2" localSheetId="4">CarriedForwards!#REF!</definedName>
     <definedName name="DateOfSale">Report!$A$7</definedName>
     <definedName name="DateOfSaleCF2" localSheetId="4">CarriedForwards!$B$7</definedName>
+    <definedName name="DCSpecialist">Report!$L$7</definedName>
     <definedName name="GrandTotalCarriedForwardPremium">Report!$C$15</definedName>
     <definedName name="GrandTotalCarriedForwardsBase">Report!$B$15</definedName>
     <definedName name="GrandTotalCarriedForwardUnits">Report!$E$15</definedName>
@@ -48,30 +49,30 @@
     <definedName name="MandateStatus">Report!$J$7</definedName>
     <definedName name="Premium">Report!$E$7</definedName>
     <definedName name="PremiumCF2" localSheetId="4">CarriedForwards!$C$7</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Report!$A$1:$X$15</definedName>
-    <definedName name="Reason">Report!$L$7</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Report!$A$1:$Y$15</definedName>
+    <definedName name="Reason">Report!$M$7</definedName>
     <definedName name="ReferralResult">Report!$I$7</definedName>
     <definedName name="RefNo">Report!$C$7</definedName>
     <definedName name="RefNoCF2" localSheetId="4">CarriedForwards!#REF!</definedName>
-    <definedName name="RPBatch">Report!$O$7</definedName>
-    <definedName name="RPCampaign">Report!$N$5</definedName>
-    <definedName name="RPClient">Report!$Q$7</definedName>
-    <definedName name="RPDateOfSale">Report!$N$7</definedName>
-    <definedName name="RPFallOffPremium">Report!$T$7</definedName>
-    <definedName name="RPGrandTotalFallOffPremium">Report!$T$10</definedName>
-    <definedName name="RPGrandTotalOriginalPremium">Report!$R$10</definedName>
-    <definedName name="RPGrandTotalReducedPremium">Report!$S$10</definedName>
-    <definedName name="RPGrandTotalSales">Report!$P$10</definedName>
-    <definedName name="RPGrandTotalUnits">Report!$U$10</definedName>
-    <definedName name="RPOriginalPremium">Report!$R$7</definedName>
-    <definedName name="RPReducedPremium">Report!$S$7</definedName>
-    <definedName name="RPRefno">Report!$P$7</definedName>
-    <definedName name="RPTotalFallOffPremium">Report!$T$8</definedName>
-    <definedName name="RPTotalOriginalPremium">Report!$R$8</definedName>
-    <definedName name="RPTotalReducedPremium">Report!$S$8</definedName>
-    <definedName name="RPTotalSales">Report!$P$8</definedName>
-    <definedName name="RPTotalUnits">Report!$U$8</definedName>
-    <definedName name="RPUnits">Report!$U$7</definedName>
+    <definedName name="RPBatch">Report!$P$7</definedName>
+    <definedName name="RPCampaign">Report!$O$5</definedName>
+    <definedName name="RPClient">Report!$R$7</definedName>
+    <definedName name="RPDateOfSale">Report!$O$7</definedName>
+    <definedName name="RPFallOffPremium">Report!$U$7</definedName>
+    <definedName name="RPGrandTotalFallOffPremium">Report!$U$10</definedName>
+    <definedName name="RPGrandTotalOriginalPremium">Report!$S$10</definedName>
+    <definedName name="RPGrandTotalReducedPremium">Report!$T$10</definedName>
+    <definedName name="RPGrandTotalSales">Report!$Q$10</definedName>
+    <definedName name="RPGrandTotalUnits">Report!$V$10</definedName>
+    <definedName name="RPOriginalPremium">Report!$S$7</definedName>
+    <definedName name="RPReducedPremium">Report!$T$7</definedName>
+    <definedName name="RPRefno">Report!$Q$7</definedName>
+    <definedName name="RPTotalFallOffPremium">Report!$U$8</definedName>
+    <definedName name="RPTotalOriginalPremium">Report!$S$8</definedName>
+    <definedName name="RPTotalReducedPremium">Report!$T$8</definedName>
+    <definedName name="RPTotalSales">Report!$Q$8</definedName>
+    <definedName name="RPTotalUnits">Report!$V$8</definedName>
+    <definedName name="RPUnits">Report!$V$7</definedName>
     <definedName name="SalesDates">Report!$A$3</definedName>
     <definedName name="SalesDatesCF">CarriedForwards!$B$3</definedName>
     <definedName name="SalesDatesCF2" localSheetId="4">CarriedForwards!$B$3</definedName>
@@ -93,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
   <si>
     <t>Reference</t>
   </si>
@@ -225,6 +226,9 @@
   </si>
   <si>
     <t>Reference Number</t>
+  </si>
+  <si>
+    <t>Forward to DC Specialist</t>
   </si>
 </sst>
 </file>
@@ -679,6 +683,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -739,14 +751,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1028,10 +1032,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U15"/>
+  <dimension ref="A1:V15"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1042,53 +1046,54 @@
     <col min="6" max="6" width="14.7265625" style="12" customWidth="1"/>
     <col min="7" max="7" width="16.7265625" customWidth="1"/>
     <col min="8" max="11" width="16.7265625" style="24" customWidth="1"/>
-    <col min="12" max="12" width="43.08984375" style="24" customWidth="1"/>
-    <col min="13" max="13" width="19.36328125" style="24" customWidth="1"/>
-    <col min="14" max="15" width="18.7265625" customWidth="1"/>
-    <col min="16" max="16" width="24.7265625" customWidth="1"/>
-    <col min="17" max="17" width="18.7265625" customWidth="1"/>
-    <col min="18" max="18" width="18.7265625" style="24" customWidth="1"/>
-    <col min="19" max="19" width="18.7265625" customWidth="1"/>
-    <col min="20" max="20" width="18.7265625" style="24" customWidth="1"/>
-    <col min="21" max="21" width="12.7265625" customWidth="1"/>
+    <col min="12" max="13" width="43.08984375" style="24" customWidth="1"/>
+    <col min="14" max="14" width="19.36328125" style="24" customWidth="1"/>
+    <col min="15" max="16" width="18.7265625" customWidth="1"/>
+    <col min="17" max="17" width="24.7265625" customWidth="1"/>
+    <col min="18" max="18" width="18.7265625" customWidth="1"/>
+    <col min="19" max="19" width="18.7265625" style="24" customWidth="1"/>
+    <col min="20" max="20" width="18.7265625" customWidth="1"/>
+    <col min="21" max="21" width="18.7265625" style="24" customWidth="1"/>
+    <col min="22" max="22" width="12.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A5" s="68" t="s">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A5" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
       <c r="I5" s="58"/>
       <c r="J5" s="66"/>
       <c r="K5" s="66"/>
-      <c r="L5" s="62"/>
-      <c r="N5" s="68" t="s">
+      <c r="L5" s="41"/>
+      <c r="M5" s="62"/>
+      <c r="O5" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="69"/>
-      <c r="P5" s="69"/>
-      <c r="Q5" s="69"/>
-      <c r="R5" s="69"/>
-      <c r="S5" s="69"/>
-      <c r="T5" s="69"/>
-      <c r="U5" s="70"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="P5" s="73"/>
+      <c r="Q5" s="73"/>
+      <c r="R5" s="73"/>
+      <c r="S5" s="73"/>
+      <c r="T5" s="73"/>
+      <c r="U5" s="73"/>
+      <c r="V5" s="74"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
@@ -1122,35 +1127,38 @@
       <c r="K6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="M6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="O6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="P6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="P6" s="7" t="s">
+      <c r="Q6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="Q6" s="7" t="s">
+      <c r="R6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="R6" s="7" t="s">
+      <c r="S6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="S6" s="7" t="s">
+      <c r="T6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="T6" s="7" t="s">
+      <c r="U6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="U6" s="7" t="s">
+      <c r="V6" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1163,16 +1171,17 @@
       <c r="J7" s="59"/>
       <c r="K7" s="59"/>
       <c r="L7" s="63"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="3"/>
+      <c r="M7" s="63"/>
+      <c r="O7" s="2"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
-      <c r="R7" s="4"/>
+      <c r="R7" s="3"/>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
-      <c r="U7" s="64"/>
-    </row>
-    <row r="8" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="U7" s="4"/>
+      <c r="V7" s="64"/>
+    </row>
+    <row r="8" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C8" s="6"/>
       <c r="E8" s="5"/>
       <c r="F8" s="14"/>
@@ -1183,24 +1192,25 @@
       <c r="J8" s="61"/>
       <c r="K8" s="60"/>
       <c r="L8" s="61"/>
-      <c r="N8" s="24"/>
+      <c r="M8" s="61"/>
       <c r="O8" s="24"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="5"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="24"/>
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
-      <c r="U8" s="65"/>
-    </row>
-    <row r="9" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="N9" s="24"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="65"/>
+    </row>
+    <row r="9" spans="1:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="O9" s="24"/>
       <c r="P9" s="24"/>
       <c r="Q9" s="24"/>
-      <c r="S9" s="24"/>
-      <c r="U9" s="25"/>
-    </row>
-    <row r="10" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="R9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="V9" s="25"/>
+    </row>
+    <row r="10" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="8" t="s">
         <v>6</v>
       </c>
@@ -1214,32 +1224,33 @@
       <c r="J10" s="61"/>
       <c r="K10" s="60"/>
       <c r="L10" s="61"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="23" t="s">
+      <c r="M10" s="61"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="10"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="24"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
-      <c r="U10" s="15"/>
-    </row>
-    <row r="11" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="U10" s="10"/>
+      <c r="V10" s="15"/>
+    </row>
+    <row r="11" spans="1:22" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="F12" s="25"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="B13" s="67" t="s">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B13" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67" t="s">
+      <c r="C13" s="71"/>
+      <c r="D13" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="67"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="E13" s="71"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14" s="24"/>
       <c r="B14" s="26" t="s">
         <v>13</v>
@@ -1254,7 +1265,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" s="27" t="s">
         <v>15</v>
       </c>
@@ -1270,7 +1281,7 @@
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="N5:U5"/>
+    <mergeCell ref="O5:V5"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1292,10 +1303,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="72"/>
+      <c r="B1" s="76"/>
       <c r="C1" s="18"/>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
@@ -1312,10 +1323,10 @@
       <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="73"/>
+      <c r="B3" s="77"/>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
@@ -1474,13 +1485,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="79"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="83"/>
     </row>
     <row r="2" spans="1:5" s="25" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31"/>
@@ -1490,27 +1501,27 @@
       <c r="E2" s="31"/>
     </row>
     <row r="3" spans="1:5" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A3" s="80"/>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
+      <c r="A3" s="84"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
     </row>
     <row r="4" spans="1:5" s="25" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:5" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A5" s="80"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
+      <c r="A5" s="84"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
     </row>
     <row r="6" spans="1:5" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="74"/>
-      <c r="B7" s="75"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="76"/>
+      <c r="A7" s="78"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="80"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
@@ -1537,13 +1548,13 @@
       <c r="E9" s="32"/>
     </row>
     <row r="10" spans="1:5" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="82"/>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82"/>
-      <c r="E10" s="83"/>
+      <c r="B10" s="86"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="87"/>
     </row>
     <row r="11" spans="1:5" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:5" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
@@ -1591,16 +1602,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.6">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="86"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="90"/>
     </row>
     <row r="2" spans="1:8" s="25" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31"/>
@@ -1612,34 +1623,34 @@
       <c r="G2" s="31"/>
     </row>
     <row r="3" spans="1:8" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A3" s="80"/>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
+      <c r="A3" s="84"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
     </row>
     <row r="4" spans="1:8" s="25" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:8" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A5" s="80"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
+      <c r="A5" s="84"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
     </row>
     <row r="6" spans="1:8" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="74"/>
-      <c r="B7" s="75"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="87"/>
+      <c r="A7" s="78"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="91"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
@@ -1678,16 +1689,16 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" s="25" customFormat="1" ht="13.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="82"/>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="87"/>
+      <c r="B10" s="86"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="91"/>
     </row>
     <row r="11" spans="1:8" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:8" s="25" customFormat="1" ht="13" x14ac:dyDescent="0.3">
@@ -1759,12 +1770,12 @@
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="87"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="91"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
@@ -1861,38 +1872,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{523127EF-725C-43E7-94D4-76A004FACF2B}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" style="92" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.81640625" style="70" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="72"/>
+      <c r="B1" s="76"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="89"/>
+      <c r="A2" s="67"/>
       <c r="B2" s="16"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="73"/>
+      <c r="B3" s="77"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="89"/>
+      <c r="A4" s="67"/>
       <c r="B4" s="16"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="90" t="s">
+      <c r="A5" s="68" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="17" t="s">
@@ -1900,7 +1911,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="91"/>
+      <c r="A6" s="69"/>
       <c r="B6" s="21"/>
     </row>
   </sheetData>

</xml_diff>